<commit_message>
Latest code for the jenkins..
Thanks,
Ajit Nakum
</commit_message>
<xml_diff>
--- a/Automation/Workspace/Odysseus_Product/src/main/java/testData/FaredepotData.xlsx
+++ b/Automation/Workspace/Odysseus_Product/src/main/java/testData/FaredepotData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15855" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17730" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,37 +67,37 @@
     <t>DataProviderWithExcel_001</t>
   </si>
   <si>
+    <t>Monish</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Luthra</t>
+  </si>
+  <si>
+    <t>ajit_nakum@odysseussolutions.com</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Arya</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Destination_Phone</t>
+  </si>
+  <si>
     <t>nyc</t>
   </si>
   <si>
-    <t>singa</t>
-  </si>
-  <si>
-    <t>Monish</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Luthra</t>
-  </si>
-  <si>
-    <t>ajit_nakum@odysseussolutions.com</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Arya</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Destination_Phone</t>
+    <t>yyz</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,10 +529,10 @@
         <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -540,43 +540,43 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O2">
         <v>8952634785</v>

</xml_diff>